<commit_message>
Get Car Price Test Task Accurate View
</commit_message>
<xml_diff>
--- a/GetCarPrice/Output/CarInfo.xlsx
+++ b/GetCarPrice/Output/CarInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <x:si>
     <x:t>Car</x:t>
   </x:si>
@@ -25,31 +25,100 @@
     <x:t>Price</x:t>
   </x:si>
   <x:si>
+    <x:t>Acura MDX 4 поколение, 7 мест</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/mdx/104666965</x:t>
+  </x:si>
+  <x:si>
+    <x:t>151 277 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura MDX II, 7 мест</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/mdx/110422144</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37 504 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura TLX II</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/tlx/110353727</x:t>
+  </x:si>
+  <x:si>
+    <x:t>113 142 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/tlx/109439353</x:t>
+  </x:si>
+  <x:si>
+    <x:t>110 306 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura ILX I · 2-й рестайлинг</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/ilx/107039143</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58 305 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura RDX III</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/rdx/110406040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>113 458 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/mdx/109423928</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40 813 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura RDX I · Рестайлинг</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/rdx/103491502</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45 068 р.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acura TLX I · Рестайлинг</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/acura/tlx/104981738</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69 335 р.</x:t>
+  </x:si>
+  <x:si>
     <x:t>Acura RDX II · Рестайлинг</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110191475</x:t>
   </x:si>
   <x:si>
-    <x:t>57 947 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura MDX II, 7 мест</x:t>
+    <x:t>57 989 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/107664244</x:t>
   </x:si>
   <x:si>
-    <x:t>39 366 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura RDX I · Рестайлинг</x:t>
+    <x:t>39 395 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110379828</x:t>
   </x:si>
   <x:si>
-    <x:t>28 029 р.</x:t>
+    <x:t>28 049 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura TLX I</x:t>
@@ -58,61 +127,55 @@
     <x:t>https://cars.av.by/acura/tlx/105176008</x:t>
   </x:si>
   <x:si>
-    <x:t>59 837 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura TLX II</x:t>
+    <x:t>59 880 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/110440280</x:t>
   </x:si>
   <x:si>
-    <x:t>103 927 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura RDX III</x:t>
+    <x:t>104 003 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110166477</x:t>
   </x:si>
   <x:si>
-    <x:t>104 872 р.</x:t>
+    <x:t>104 948 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/104280825</x:t>
   </x:si>
   <x:si>
-    <x:t>105 502 р.</x:t>
+    <x:t>105 579 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/101964526</x:t>
   </x:si>
   <x:si>
-    <x:t>121 248 р.</x:t>
+    <x:t>121 337 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/108357377</x:t>
   </x:si>
   <x:si>
-    <x:t>42 043 р.</x:t>
+    <x:t>42 074 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/100715989</x:t>
   </x:si>
   <x:si>
-    <x:t>40 941 р.</x:t>
+    <x:t>40 971 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/109429997</x:t>
   </x:si>
   <x:si>
-    <x:t>105 816 р.</x:t>
+    <x:t>105 894 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/108357609</x:t>
   </x:si>
   <x:si>
-    <x:t>102 352 р.</x:t>
+    <x:t>102 427 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura TSX I</x:t>
@@ -121,7 +184,7 @@
     <x:t>https://cars.av.by/acura/tsx/110211579</x:t>
   </x:si>
   <x:si>
-    <x:t>20 470 р.</x:t>
+    <x:t>20 485 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura TSX II</x:t>
@@ -130,7 +193,7 @@
     <x:t>https://cars.av.by/acura/tsx/100994111</x:t>
   </x:si>
   <x:si>
-    <x:t>33 383 р.</x:t>
+    <x:t>33 407 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura TL IV</x:t>
@@ -139,31 +202,31 @@
     <x:t>https://cars.av.by/acura/tl/109185697</x:t>
   </x:si>
   <x:si>
-    <x:t>42 201 р.</x:t>
+    <x:t>42 231 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/110337283</x:t>
   </x:si>
   <x:si>
-    <x:t>64 561 р.</x:t>
+    <x:t>64 608 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110458349</x:t>
   </x:si>
   <x:si>
-    <x:t>83 142 р.</x:t>
+    <x:t>83 202 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/109427439</x:t>
   </x:si>
   <x:si>
-    <x:t>110 222 р.</x:t>
+    <x:t>110 303 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/109621548</x:t>
   </x:si>
   <x:si>
-    <x:t>38 736 р.</x:t>
+    <x:t>38 765 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura MDX II · Рестайлинг, 7 мест</x:t>
@@ -172,7 +235,7 @@
     <x:t>https://cars.av.by/acura/mdx/109202038</x:t>
   </x:si>
   <x:si>
-    <x:t>50 389 р.</x:t>
+    <x:t>50 426 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/110463467</x:t>
@@ -181,7 +244,7 @@
     <x:t>https://cars.av.by/acura/mdx/108961451</x:t>
   </x:si>
   <x:si>
-    <x:t>38 107 р.</x:t>
+    <x:t>38 134 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura ILX I</x:t>
@@ -190,7 +253,7 @@
     <x:t>https://cars.av.by/acura/ilx/109708460</x:t>
   </x:si>
   <x:si>
-    <x:t>33 698 р.</x:t>
+    <x:t>33 722 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura MDX I, 7 мест</x:t>
@@ -199,139 +262,94 @@
     <x:t>https://cars.av.by/acura/mdx/110386886</x:t>
   </x:si>
   <x:si>
+    <x:t>19 540 р.</x:t>
+  </x:si>
+  <x:si>
     <x:t>Acura Integra IV</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/integra/109291376</x:t>
   </x:si>
   <x:si>
-    <x:t>100 463 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura TLX I · Рестайлинг</x:t>
+    <x:t>100 536 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/110221816</x:t>
   </x:si>
   <x:si>
-    <x:t>69 285 р.</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://cars.av.by/acura/rdx/108640327</x:t>
   </x:si>
   <x:si>
-    <x:t>42 358 р.</x:t>
+    <x:t>42 389 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/108417623</x:t>
   </x:si>
   <x:si>
-    <x:t>100 778 р.</x:t>
+    <x:t>100 851 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110215862</x:t>
   </x:si>
   <x:si>
-    <x:t>50 386 р.</x:t>
+    <x:t>50 422 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/100811580</x:t>
   </x:si>
   <x:si>
-    <x:t>110 226 р.</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://cars.av.by/acura/tlx/107287966</x:t>
   </x:si>
   <x:si>
-    <x:t>91 330 р.</x:t>
+    <x:t>91 396 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/107480084</x:t>
   </x:si>
   <x:si>
-    <x:t>Acura ILX I · 2-й рестайлинг</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/ilx/107039143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>58 262 р.</x:t>
-  </x:si>
-  <x:si>
     <x:t>Acura RDX II</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110354958</x:t>
   </x:si>
   <x:si>
-    <x:t>55 113 р.</x:t>
+    <x:t>55 153 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/106382926</x:t>
   </x:si>
   <x:si>
-    <x:t>44 090 р.</x:t>
+    <x:t>44 122 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/109287380</x:t>
   </x:si>
   <x:si>
-    <x:t>94 479 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/mdx/109423928</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40 783 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura MDX 4 поколение, 7 мест</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/mdx/104666965</x:t>
-  </x:si>
-  <x:si>
-    <x:t>151 166 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/rdx/110406040</x:t>
-  </x:si>
-  <x:si>
-    <x:t>113 375 р.</x:t>
+    <x:t>94 548 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110399976</x:t>
   </x:si>
   <x:si>
-    <x:t>95 424 р.</x:t>
+    <x:t>95 493 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/110182429</x:t>
   </x:si>
   <x:si>
-    <x:t>24 250 р.</x:t>
+    <x:t>24 267 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110121787</x:t>
   </x:si>
   <x:si>
-    <x:t>40 626 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/tlx/109439353</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/rdx/103491502</x:t>
-  </x:si>
-  <x:si>
-    <x:t>45 035 р.</x:t>
+    <x:t>40 656 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tsx/110180434</x:t>
   </x:si>
   <x:si>
-    <x:t>29 392 р.</x:t>
+    <x:t>29 414 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura MDX II · Рестайлинг</x:t>
@@ -343,31 +361,31 @@
     <x:t>https://cars.av.by/acura/tsx/107047785</x:t>
   </x:si>
   <x:si>
-    <x:t>25 824 р.</x:t>
+    <x:t>25 843 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110136992</x:t>
   </x:si>
   <x:si>
-    <x:t>111 800 р.</x:t>
+    <x:t>111 882 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/104687835</x:t>
   </x:si>
   <x:si>
-    <x:t>61 411 р.</x:t>
+    <x:t>61 456 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/108351408</x:t>
   </x:si>
   <x:si>
-    <x:t>58 577 р.</x:t>
+    <x:t>58 620 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/110142219</x:t>
   </x:si>
   <x:si>
-    <x:t>11 023 р.</x:t>
+    <x:t>11 031 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura TL III</x:t>
@@ -376,13 +394,13 @@
     <x:t>https://cars.av.by/acura/tl/110411628</x:t>
   </x:si>
   <x:si>
-    <x:t>18 581 р.</x:t>
+    <x:t>18 594 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/110336980</x:t>
   </x:si>
   <x:si>
-    <x:t>107 073 р.</x:t>
+    <x:t>107 151 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura CL I</x:t>
@@ -391,7 +409,7 @@
     <x:t>https://cars.av.by/acura/cl/102580126</x:t>
   </x:si>
   <x:si>
-    <x:t>10 393 р.</x:t>
+    <x:t>10 400 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Acura MDX III · 2-й рестайлинг, 7 мест</x:t>
@@ -400,7 +418,7 @@
     <x:t>https://cars.av.by/acura/mdx/102191065</x:t>
   </x:si>
   <x:si>
-    <x:t>122 508 р.</x:t>
+    <x:t>122 597 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/108446896</x:t>
@@ -412,7 +430,7 @@
     <x:t>https://cars.av.by/acura/rdx/109343432</x:t>
   </x:si>
   <x:si>
-    <x:t>29 918 р.</x:t>
+    <x:t>29 940 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/110372698</x:t>
@@ -421,25 +439,13 @@
     <x:t>https://cars.av.by/acura/integra/110433032</x:t>
   </x:si>
   <x:si>
-    <x:t>94 164 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/tlx/110353727</x:t>
-  </x:si>
-  <x:si>
-    <x:t>113 060 р.</x:t>
+    <x:t>94 233 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/109906111</x:t>
   </x:si>
   <x:si>
-    <x:t>75 583 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/mdx/110422144</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37 477 р.</x:t>
+    <x:t>75 638 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/integra/110321801</x:t>
@@ -448,13 +454,13 @@
     <x:t>https://cars.av.by/acura/tsx/109148242</x:t>
   </x:si>
   <x:si>
-    <x:t>28 344 р.</x:t>
+    <x:t>28 364 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/tlx/110448484</x:t>
   </x:si>
   <x:si>
-    <x:t>51 963 р.</x:t>
+    <x:t>52 001 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/106855193</x:t>
@@ -466,7 +472,7 @@
     <x:t>https://cars.av.by/acura/mdx/109320248</x:t>
   </x:si>
   <x:si>
-    <x:t>69 281 р.</x:t>
+    <x:t>69 332 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/ilx/109630033</x:t>
@@ -475,34 +481,25 @@
     <x:t>https://cars.av.by/acura/mdx/107217408</x:t>
   </x:si>
   <x:si>
-    <x:t>94 385 р.</x:t>
+    <x:t>94 453 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/rdx/108277663</x:t>
   </x:si>
   <x:si>
-    <x:t>78 418 р.</x:t>
+    <x:t>78 475 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/104915189</x:t>
   </x:si>
   <x:si>
-    <x:t>43 933 р.</x:t>
+    <x:t>43 965 р.</x:t>
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/acura/mdx/104112574</x:t>
   </x:si>
   <x:si>
-    <x:t>106 446 р.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acura RDX III · Рестайлинг</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/acura/rdx/107416798</x:t>
-  </x:si>
-  <x:si>
-    <x:t>137 624 р.</x:t>
+    <x:t>106 524 р.</x:t>
   </x:si>
   <x:si>
     <x:t>Kia Cee'd III</x:t>
@@ -923,51 +920,51 @@
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
+      <x:c r="C7" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>23</x:v>
@@ -978,73 +975,73 @@
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>40</x:v>
@@ -1055,7 +1052,7 @@
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
         <x:v>42</x:v>
@@ -1066,7 +1063,7 @@
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>44</x:v>
@@ -1077,7 +1074,7 @@
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
         <x:v>46</x:v>
@@ -1099,73 +1096,73 @@
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
+      <x:c r="C21" s="0" t="s">
         <x:v>51</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
         <x:v>65</x:v>
@@ -1176,7 +1173,7 @@
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
         <x:v>67</x:v>
@@ -1187,7 +1184,7 @@
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
         <x:v>69</x:v>
@@ -1198,29 +1195,29 @@
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
         <x:v>75</x:v>
@@ -1231,73 +1228,73 @@
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
         <x:v>91</x:v>
@@ -1308,62 +1305,62 @@
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
         <x:v>93</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
         <x:v>95</x:v>
-      </x:c>
-      <x:c r="C41" s="0" t="s">
-        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
         <x:v>99</x:v>
-      </x:c>
-      <x:c r="C43" s="0" t="s">
-        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
         <x:v>101</x:v>
-      </x:c>
-      <x:c r="C44" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
         <x:v>102</x:v>
@@ -1374,7 +1371,7 @@
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
         <x:v>104</x:v>
@@ -1385,18 +1382,18 @@
     </x:row>
     <x:row r="47" spans="1:3">
       <x:c r="A47" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
-      <x:c r="B47" s="0" t="s">
+      <x:c r="C47" s="0" t="s">
         <x:v>107</x:v>
-      </x:c>
-      <x:c r="C47" s="0" t="s">
-        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
         <x:v>108</x:v>
@@ -1407,7 +1404,7 @@
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
         <x:v>110</x:v>
@@ -1418,18 +1415,18 @@
     </x:row>
     <x:row r="50" spans="1:3">
       <x:c r="A50" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:3">
       <x:c r="A51" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
         <x:v>114</x:v>
@@ -1440,7 +1437,7 @@
     </x:row>
     <x:row r="52" spans="1:3">
       <x:c r="A52" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
         <x:v>116</x:v>
@@ -1451,117 +1448,117 @@
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
         <x:v>118</x:v>
       </x:c>
-      <x:c r="B53" s="0" t="s">
+      <x:c r="C53" s="0" t="s">
         <x:v>119</x:v>
-      </x:c>
-      <x:c r="C53" s="0" t="s">
-        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
         <x:v>121</x:v>
-      </x:c>
-      <x:c r="C54" s="0" t="s">
-        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
         <x:v>123</x:v>
-      </x:c>
-      <x:c r="B55" s="0" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="C55" s="0" t="s">
-        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:3">
       <x:c r="A56" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
         <x:v>126</x:v>
-      </x:c>
-      <x:c r="B56" s="0" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="C56" s="0" t="s">
-        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:3">
       <x:c r="A57" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="B58" s="0" t="s">
+      <x:c r="C58" s="0" t="s">
         <x:v>131</x:v>
-      </x:c>
-      <x:c r="C58" s="0" t="s">
-        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
         <x:v>133</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:3">
       <x:c r="A60" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:3">
       <x:c r="A61" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:3">
       <x:c r="A62" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:3">
       <x:c r="A63" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
         <x:v>140</x:v>
@@ -1572,29 +1569,29 @@
     </x:row>
     <x:row r="64" spans="1:3">
       <x:c r="A64" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
         <x:v>142</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:3">
       <x:c r="A65" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:3">
       <x:c r="A66" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
         <x:v>145</x:v>
@@ -1605,51 +1602,51 @@
     </x:row>
     <x:row r="67" spans="1:3">
       <x:c r="A67" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
         <x:v>147</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:3">
       <x:c r="A68" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
         <x:v>149</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:3">
       <x:c r="A69" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
         <x:v>151</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:3">
       <x:c r="A70" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:3">
       <x:c r="A71" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
         <x:v>154</x:v>
@@ -1660,7 +1657,7 @@
     </x:row>
     <x:row r="72" spans="1:3">
       <x:c r="A72" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
         <x:v>156</x:v>
@@ -1671,7 +1668,7 @@
     </x:row>
     <x:row r="73" spans="1:3">
       <x:c r="A73" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
         <x:v>158</x:v>
@@ -1682,35 +1679,35 @@
     </x:row>
     <x:row r="74" spans="1:3">
       <x:c r="A74" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="B74" s="0" t="s">
+      <x:c r="C74" s="0" t="s">
         <x:v>161</x:v>
-      </x:c>
-      <x:c r="C74" s="0" t="s">
-        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:3">
       <x:c r="A75" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
         <x:v>163</x:v>
       </x:c>
-      <x:c r="B75" s="0" t="s">
+      <x:c r="C75" s="0" t="s">
         <x:v>164</x:v>
-      </x:c>
-      <x:c r="C75" s="0" t="s">
-        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:3">
       <x:c r="A76" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
-      <x:c r="B76" s="0" t="s">
+      <x:c r="C76" s="0" t="s">
         <x:v>167</x:v>
-      </x:c>
-      <x:c r="C76" s="0" t="s">
-        <x:v>168</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>